<commit_message>
added iterations and structured
</commit_message>
<xml_diff>
--- a/src/test/java/com/team1/xlImport/data.xlsx
+++ b/src/test/java/com/team1/xlImport/data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>id</t>
   </si>
@@ -46,6 +46,18 @@
   </si>
   <si>
     <t>na</t>
+  </si>
+  <si>
+    <t>rock45@phptravels.com</t>
+  </si>
+  <si>
+    <t>ramco</t>
+  </si>
+  <si>
+    <t>bunny@phptravels.com</t>
+  </si>
+  <si>
+    <t>dessert</t>
   </si>
 </sst>
 </file>
@@ -380,10 +392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,10 +446,40 @@
         <v>8</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>103</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>104</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
     <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>